<commit_message>
Fixed auto increment on the entity classes
</commit_message>
<xml_diff>
--- a/Sprint reports.xlsx
+++ b/Sprint reports.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\OneDrive\Documents\Studie\2nd year\IDATA2301_Web\GroupProject\WebApplicationProject2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{0E49F6F7-3CEA-43DA-B9E3-0AAE008F7102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8442A2-1650-47F7-95D8-CC1DED489B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,7 +106,7 @@
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-414]d/\ mmm\.\ yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -737,22 +737,22 @@
   </sheetPr>
   <dimension ref="B1:E16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="30" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.69921875" customWidth="1"/>
-    <col min="2" max="2" width="15.69921875" customWidth="1"/>
-    <col min="3" max="3" width="30.69921875" customWidth="1"/>
-    <col min="4" max="4" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="53.59765625" customWidth="1"/>
-    <col min="6" max="6" width="2.69921875" customWidth="1"/>
-    <col min="8" max="8" width="9.09765625" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="15.7265625" customWidth="1"/>
+    <col min="3" max="3" width="30.7265625" customWidth="1"/>
+    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.6328125" customWidth="1"/>
+    <col min="6" max="6" width="2.7265625" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -760,8 +760,8 @@
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:5" ht="15" customHeight="1"/>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
@@ -771,7 +771,7 @@
       </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1">
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
@@ -781,8 +781,8 @@
       </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" ht="15" customHeight="1"/>
+    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
@@ -790,7 +790,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -804,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B8" s="3">
         <v>1</v>
       </c>
@@ -814,9 +814,9 @@
       <c r="D8" s="4"/>
       <c r="E8"/>
     </row>
-    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B9" s="3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -824,9 +824,9 @@
       <c r="D9" s="4"/>
       <c r="E9"/>
     </row>
-    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B10" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -834,9 +834,9 @@
       <c r="D10" s="4"/>
       <c r="E10"/>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B11" s="3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -844,9 +844,9 @@
       <c r="D11" s="4"/>
       <c r="E11"/>
     </row>
-    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B12" s="3">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -854,9 +854,9 @@
       <c r="D12" s="4"/>
       <c r="E12"/>
     </row>
-    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B13" s="3">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -864,9 +864,9 @@
       <c r="D13" s="4"/>
       <c r="E13"/>
     </row>
-    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B14" s="3">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C14" t="s">
         <v>15</v>
@@ -874,9 +874,9 @@
       <c r="D14" s="4"/>
       <c r="E14"/>
     </row>
-    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B15" s="3">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -884,7 +884,7 @@
       <c r="D15" s="4"/>
       <c r="E15"/>
     </row>
-    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1">
       <c r="B16" s="3">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Some changes to the sprint report
</commit_message>
<xml_diff>
--- a/Sprint reports.xlsx
+++ b/Sprint reports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakob\OneDrive\Documents\Studie\2nd year\IDATA2301_Web\GroupProject\WebApplicationProject2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07BF561F-FD1C-4022-AF13-943CCD0F1379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB88233-7B4D-43F6-9E52-5842789C4E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProFLex Sprints" sheetId="1" r:id="rId1"/>
@@ -765,7 +765,7 @@
   <dimension ref="B1:E16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="30" customHeight="1"/>
@@ -817,7 +817,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="15">
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="14">
       <c r="B7" t="s">
         <v>3</v>
       </c>

</xml_diff>